<commit_message>
Se incluyen histogramas de CR para 1 sec, 1 min, 15 min, 30 min y 1 hora, por cada canal en el archivo de Configuracion xlsx de GASIFIC
</commit_message>
<xml_diff>
--- a/calibration/Test4det/Test4det_archivo_calibracion.xlsx
+++ b/calibration/Test4det/Test4det_archivo_calibracion.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="145">
   <si>
     <t>Modules</t>
   </si>
@@ -356,15 +356,33 @@
     <t>Rate units</t>
   </si>
   <si>
+    <t>ch1_12cm_fast_CR_1sec</t>
+  </si>
+  <si>
+    <t>TimeEL</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>1 sec</t>
+  </si>
+  <si>
+    <t>Counts per 1 sec</t>
+  </si>
+  <si>
+    <t>ch1_12cm_fast_CR_1min</t>
+  </si>
+  <si>
+    <t>1 min</t>
+  </si>
+  <si>
+    <t>Counts per 1 min</t>
+  </si>
+  <si>
     <t>ch1_12cm_fast_CR_15min</t>
   </si>
   <si>
-    <t>TimeEL</t>
-  </si>
-  <si>
-    <t>Timestamp</t>
-  </si>
-  <si>
     <t>15 min</t>
   </si>
   <si>
@@ -389,6 +407,12 @@
     <t>Counts per 1 hour</t>
   </si>
   <si>
+    <t>ch2_6cm_epi_CR_1sec</t>
+  </si>
+  <si>
+    <t>ch2_6cm_epi_CR_1min</t>
+  </si>
+  <si>
     <t>ch2_6cm_epi_CR_15min</t>
   </si>
   <si>
@@ -398,6 +422,12 @@
     <t>ch2_6cm_epi_CR_1h</t>
   </si>
   <si>
+    <t>ch3_pb_HE_CR_1sec</t>
+  </si>
+  <si>
+    <t>ch3_pb_HE_CR_1min</t>
+  </si>
+  <si>
     <t>ch3_pb_HE_CR_15min</t>
   </si>
   <si>
@@ -405,6 +435,12 @@
   </si>
   <si>
     <t>ch3_pb_HE_CR_1h</t>
+  </si>
+  <si>
+    <t>ch4_naked_th_CR_1sec</t>
+  </si>
+  <si>
+    <t>ch4_naked_th_CR_1min</t>
   </si>
   <si>
     <t>ch4_naked_th_CR_15min</t>
@@ -871,10 +907,6 @@
       <c r="I3">
         <v>1000000</v>
       </c>
-      <c r="J3" t="e">
-        <f>#NUM!</f>
-        <v>#NUM!</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1969,10 +2001,10 @@
         <v>15000</v>
       </c>
       <c r="I3">
-        <v>0.0467447368421052</v>
+        <v>0.0465513103448275</v>
       </c>
       <c r="J3">
-        <v>-34.39058171745157</v>
+        <v>-34.24827586206894</v>
       </c>
       <c r="K3" t="s">
         <v>97</v>
@@ -2004,10 +2036,10 @@
         <v>15000</v>
       </c>
       <c r="I4">
-        <v>0.0432688461538461</v>
+        <v>0.0429932484076433</v>
       </c>
       <c r="J4">
-        <v>-27.18076923076924</v>
+        <v>-27.98089171974522</v>
       </c>
       <c r="K4" t="s">
         <v>97</v>
@@ -2039,10 +2071,10 @@
         <v>15000</v>
       </c>
       <c r="I5">
-        <v>0.0238513780918727</v>
+        <v>0.023684</v>
       </c>
       <c r="J5">
-        <v>-39.81978798586567</v>
+        <v>-36.18947368421053</v>
       </c>
       <c r="K5" t="s">
         <v>97</v>
@@ -2074,10 +2106,10 @@
         <v>15000</v>
       </c>
       <c r="I6">
-        <v>0.0248342163355408</v>
+        <v>0.0248159558823529</v>
       </c>
       <c r="J6">
-        <v>-23.40066225165566</v>
+        <v>-23.87499999999994</v>
       </c>
       <c r="K6" t="s">
         <v>97</v>
@@ -2093,7 +2125,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:O36"/>
+  <dimension ref="B1:O60"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2171,13 +2203,13 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>10000</v>
+        <v>600000</v>
       </c>
       <c r="J3">
-        <v>10000</v>
+        <v>600000</v>
       </c>
       <c r="K3">
-        <v>1.777777777777778E-10</v>
+        <v>1.6E-07</v>
       </c>
       <c r="L3" t="s">
         <v>115</v>
@@ -2264,13 +2296,13 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>5000</v>
+        <v>100000</v>
       </c>
       <c r="J6">
-        <v>5000</v>
+        <v>100000</v>
       </c>
       <c r="K6">
-        <v>8.888888888888889E-11</v>
+        <v>2.666666666666667E-09</v>
       </c>
       <c r="L6" t="s">
         <v>118</v>
@@ -2357,13 +2389,13 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>2500</v>
+        <v>10000</v>
       </c>
       <c r="J9">
-        <v>2500</v>
+        <v>10000</v>
       </c>
       <c r="K9">
-        <v>4.444444444444444E-11</v>
+        <v>1.777777777777778E-10</v>
       </c>
       <c r="L9" t="s">
         <v>121</v>
@@ -2435,7 +2467,7 @@
         <v>113</v>
       </c>
       <c r="D12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E12">
         <v>140</v>
@@ -2450,16 +2482,16 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="J12">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="K12">
-        <v>1.777777777777778E-10</v>
+        <v>8.888888888888889E-11</v>
       </c>
       <c r="L12" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="M12">
         <v>1</v>
@@ -2468,7 +2500,7 @@
         <v>1</v>
       </c>
       <c r="O12" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="2:15">
@@ -2522,13 +2554,13 @@
     </row>
     <row r="15" spans="2:15">
       <c r="B15" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C15" t="s">
         <v>113</v>
       </c>
       <c r="D15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E15">
         <v>140</v>
@@ -2543,16 +2575,16 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="J15">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="K15">
-        <v>8.888888888888889E-11</v>
+        <v>4.444444444444444E-11</v>
       </c>
       <c r="L15" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="M15">
         <v>1</v>
@@ -2561,7 +2593,7 @@
         <v>1</v>
       </c>
       <c r="O15" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="2:15">
@@ -2615,7 +2647,7 @@
     </row>
     <row r="18" spans="2:15">
       <c r="B18" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C18" t="s">
         <v>113</v>
@@ -2636,16 +2668,16 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>2500</v>
+        <v>600000</v>
       </c>
       <c r="J18">
-        <v>2500</v>
+        <v>600000</v>
       </c>
       <c r="K18">
-        <v>4.444444444444444E-11</v>
+        <v>1.6E-07</v>
       </c>
       <c r="L18" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="M18">
         <v>1</v>
@@ -2654,7 +2686,7 @@
         <v>1</v>
       </c>
       <c r="O18" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="2:15">
@@ -2708,13 +2740,13 @@
     </row>
     <row r="21" spans="2:15">
       <c r="B21" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C21" t="s">
         <v>113</v>
       </c>
       <c r="D21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E21">
         <v>140</v>
@@ -2729,16 +2761,16 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="J21">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="K21">
-        <v>1.777777777777778E-10</v>
+        <v>2.666666666666667E-09</v>
       </c>
       <c r="L21" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="M21">
         <v>1</v>
@@ -2747,7 +2779,7 @@
         <v>1</v>
       </c>
       <c r="O21" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="2:15">
@@ -2801,13 +2833,13 @@
     </row>
     <row r="24" spans="2:15">
       <c r="B24" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C24" t="s">
         <v>113</v>
       </c>
       <c r="D24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E24">
         <v>140</v>
@@ -2822,16 +2854,16 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="J24">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="K24">
-        <v>8.888888888888889E-11</v>
+        <v>1.777777777777778E-10</v>
       </c>
       <c r="L24" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -2840,7 +2872,7 @@
         <v>1</v>
       </c>
       <c r="O24" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="2:15">
@@ -2894,13 +2926,13 @@
     </row>
     <row r="27" spans="2:15">
       <c r="B27" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C27" t="s">
         <v>113</v>
       </c>
       <c r="D27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E27">
         <v>140</v>
@@ -2915,16 +2947,16 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="J27">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="K27">
-        <v>4.444444444444444E-11</v>
+        <v>8.888888888888889E-11</v>
       </c>
       <c r="L27" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="M27">
         <v>1</v>
@@ -2933,7 +2965,7 @@
         <v>1</v>
       </c>
       <c r="O27" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="2:15">
@@ -2987,13 +3019,13 @@
     </row>
     <row r="30" spans="2:15">
       <c r="B30" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C30" t="s">
         <v>113</v>
       </c>
       <c r="D30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E30">
         <v>140</v>
@@ -3008,16 +3040,16 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <v>10000</v>
+        <v>2500</v>
       </c>
       <c r="J30">
-        <v>10000</v>
+        <v>2500</v>
       </c>
       <c r="K30">
-        <v>1.777777777777778E-10</v>
+        <v>4.444444444444444E-11</v>
       </c>
       <c r="L30" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="M30">
         <v>1</v>
@@ -3026,7 +3058,7 @@
         <v>1</v>
       </c>
       <c r="O30" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="2:15">
@@ -3080,13 +3112,13 @@
     </row>
     <row r="33" spans="2:15">
       <c r="B33" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C33" t="s">
         <v>113</v>
       </c>
       <c r="D33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E33">
         <v>140</v>
@@ -3101,16 +3133,16 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>5000</v>
+        <v>600000</v>
       </c>
       <c r="J33">
-        <v>5000</v>
+        <v>600000</v>
       </c>
       <c r="K33">
-        <v>8.888888888888889E-11</v>
+        <v>1.6E-07</v>
       </c>
       <c r="L33" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="M33">
         <v>1</v>
@@ -3119,7 +3151,7 @@
         <v>1</v>
       </c>
       <c r="O33" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="2:15">
@@ -3173,13 +3205,13 @@
     </row>
     <row r="36" spans="2:15">
       <c r="B36" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C36" t="s">
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E36">
         <v>140</v>
@@ -3194,25 +3226,769 @@
         <v>0</v>
       </c>
       <c r="I36">
+        <v>100000</v>
+      </c>
+      <c r="J36">
+        <v>100000</v>
+      </c>
+      <c r="K36">
+        <v>2.666666666666667E-09</v>
+      </c>
+      <c r="L36" t="s">
+        <v>118</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15">
+      <c r="C37" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15">
+      <c r="B38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O38" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15">
+      <c r="B39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" t="s">
+        <v>99</v>
+      </c>
+      <c r="E39">
+        <v>140</v>
+      </c>
+      <c r="F39">
+        <v>820</v>
+      </c>
+      <c r="G39" t="s">
+        <v>114</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>10000</v>
+      </c>
+      <c r="J39">
+        <v>10000</v>
+      </c>
+      <c r="K39">
+        <v>1.777777777777778E-10</v>
+      </c>
+      <c r="L39" t="s">
+        <v>121</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
+      <c r="O39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15">
+      <c r="C40" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15">
+      <c r="B41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O41" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15">
+      <c r="B42" t="s">
+        <v>137</v>
+      </c>
+      <c r="C42" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" t="s">
+        <v>99</v>
+      </c>
+      <c r="E42">
+        <v>140</v>
+      </c>
+      <c r="F42">
+        <v>820</v>
+      </c>
+      <c r="G42" t="s">
+        <v>114</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>5000</v>
+      </c>
+      <c r="J42">
+        <v>5000</v>
+      </c>
+      <c r="K42">
+        <v>8.888888888888889E-11</v>
+      </c>
+      <c r="L42" t="s">
+        <v>124</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15">
+      <c r="C43" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15">
+      <c r="B44" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O44" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15">
+      <c r="B45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45" t="s">
+        <v>99</v>
+      </c>
+      <c r="E45">
+        <v>140</v>
+      </c>
+      <c r="F45">
+        <v>820</v>
+      </c>
+      <c r="G45" t="s">
+        <v>114</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
         <v>2500</v>
       </c>
-      <c r="J36">
+      <c r="J45">
         <v>2500</v>
       </c>
-      <c r="K36">
+      <c r="K45">
         <v>4.444444444444444E-11</v>
       </c>
-      <c r="L36" t="s">
+      <c r="L45" t="s">
+        <v>127</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
+      <c r="O45" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15">
+      <c r="C46" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15">
+      <c r="B47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O47" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15">
+      <c r="B48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" t="s">
+        <v>113</v>
+      </c>
+      <c r="D48" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48">
+        <v>140</v>
+      </c>
+      <c r="F48">
+        <v>820</v>
+      </c>
+      <c r="G48" t="s">
+        <v>114</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>600000</v>
+      </c>
+      <c r="J48">
+        <v>600000</v>
+      </c>
+      <c r="K48">
+        <v>1.6E-07</v>
+      </c>
+      <c r="L48" t="s">
+        <v>115</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
+      <c r="O48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15">
+      <c r="C49" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15">
+      <c r="B50" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M50" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N50" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O50" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15">
+      <c r="B51" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51" t="s">
+        <v>113</v>
+      </c>
+      <c r="D51" t="s">
+        <v>100</v>
+      </c>
+      <c r="E51">
+        <v>140</v>
+      </c>
+      <c r="F51">
+        <v>820</v>
+      </c>
+      <c r="G51" t="s">
+        <v>114</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>100000</v>
+      </c>
+      <c r="J51">
+        <v>100000</v>
+      </c>
+      <c r="K51">
+        <v>2.666666666666667E-09</v>
+      </c>
+      <c r="L51" t="s">
+        <v>118</v>
+      </c>
+      <c r="M51">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+      <c r="O51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15">
+      <c r="C52" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15">
+      <c r="B53" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N53" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O53" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15">
+      <c r="B54" t="s">
+        <v>141</v>
+      </c>
+      <c r="C54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" t="s">
+        <v>100</v>
+      </c>
+      <c r="E54">
+        <v>140</v>
+      </c>
+      <c r="F54">
+        <v>820</v>
+      </c>
+      <c r="G54" t="s">
+        <v>114</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>10000</v>
+      </c>
+      <c r="J54">
+        <v>10000</v>
+      </c>
+      <c r="K54">
+        <v>1.777777777777778E-10</v>
+      </c>
+      <c r="L54" t="s">
         <v>121</v>
       </c>
-      <c r="M36">
-        <v>1</v>
-      </c>
-      <c r="N36">
-        <v>1</v>
-      </c>
-      <c r="O36" t="s">
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15">
+      <c r="C55" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15">
+      <c r="B56" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M56" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N56" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O56" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15">
+      <c r="B57" t="s">
+        <v>142</v>
+      </c>
+      <c r="C57" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" t="s">
+        <v>100</v>
+      </c>
+      <c r="E57">
+        <v>140</v>
+      </c>
+      <c r="F57">
+        <v>820</v>
+      </c>
+      <c r="G57" t="s">
+        <v>114</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>5000</v>
+      </c>
+      <c r="J57">
+        <v>5000</v>
+      </c>
+      <c r="K57">
+        <v>8.888888888888889E-11</v>
+      </c>
+      <c r="L57" t="s">
+        <v>124</v>
+      </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <v>1</v>
+      </c>
+      <c r="O57" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15">
+      <c r="C58" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="2:15">
+      <c r="B59" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K59" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M59" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N59" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O59" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="2:15">
+      <c r="B60" t="s">
+        <v>143</v>
+      </c>
+      <c r="C60" t="s">
+        <v>113</v>
+      </c>
+      <c r="D60" t="s">
+        <v>100</v>
+      </c>
+      <c r="E60">
+        <v>140</v>
+      </c>
+      <c r="F60">
+        <v>820</v>
+      </c>
+      <c r="G60" t="s">
+        <v>114</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>2500</v>
+      </c>
+      <c r="J60">
+        <v>2500</v>
+      </c>
+      <c r="K60">
+        <v>4.444444444444444E-11</v>
+      </c>
+      <c r="L60" t="s">
+        <v>127</v>
+      </c>
+      <c r="M60">
+        <v>1</v>
+      </c>
+      <c r="N60">
+        <v>1</v>
+      </c>
+      <c r="O60" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3230,7 +4006,7 @@
   <sheetData>
     <row r="1" spans="3:3">
       <c r="C1" s="1" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se puede generar archivo de configuracion para analisis offline en base ms/us para la transformacion de DLT a ROOT usando el DTASOffline del IFIC, luego de generar el xlsx
</commit_message>
<xml_diff>
--- a/calibration/Test4det/Test4det_archivo_calibracion.xlsx
+++ b/calibration/Test4det/Test4det_archivo_calibracion.xlsx
@@ -2001,10 +2001,10 @@
         <v>15000</v>
       </c>
       <c r="I3">
-        <v>0.0465513103448275</v>
+        <v>0.0467447368421052</v>
       </c>
       <c r="J3">
-        <v>-34.24827586206894</v>
+        <v>-34.39058171745157</v>
       </c>
       <c r="K3" t="s">
         <v>97</v>
@@ -2036,10 +2036,10 @@
         <v>15000</v>
       </c>
       <c r="I4">
-        <v>0.0429932484076433</v>
+        <v>0.0432688461538461</v>
       </c>
       <c r="J4">
-        <v>-27.98089171974522</v>
+        <v>-27.18076923076924</v>
       </c>
       <c r="K4" t="s">
         <v>97</v>
@@ -2071,10 +2071,10 @@
         <v>15000</v>
       </c>
       <c r="I5">
-        <v>0.023684</v>
+        <v>0.0238513780918727</v>
       </c>
       <c r="J5">
-        <v>-36.18947368421053</v>
+        <v>-39.81978798586567</v>
       </c>
       <c r="K5" t="s">
         <v>97</v>
@@ -2106,10 +2106,10 @@
         <v>15000</v>
       </c>
       <c r="I6">
-        <v>0.0248159558823529</v>
+        <v>0.0248342163355408</v>
       </c>
       <c r="J6">
-        <v>-23.87499999999994</v>
+        <v>-23.40066225165566</v>
       </c>
       <c r="K6" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
Se agregan los valores geomagneticos del lugar al crear una nueva campanya, usando PyIGRF que toma los valores de Campo Magnetico de IGRF-13 (2021). Se agrega un metodo en utils.py para seleccion de todos los detectores. En el reporte se agrega la nueva informacion de valores geograficos y geomagneticos incluyendo un enlace a google maps con la Latitud y Longitud. Se mejora recalibrate para poder seleccionar solo aquellos detectores que hayan perdido la calibracion y generar un nuevo archivo de calibracion manteniendo que modifica solo los detectores descalibrados.
</commit_message>
<xml_diff>
--- a/calibration/Test4det/Test4det_archivo_calibracion.xlsx
+++ b/calibration/Test4det/Test4det_archivo_calibracion.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
-    <sheet name="Hard_Sis3316_125_0xCC" sheetId="2" r:id="rId2"/>
-    <sheet name="Cal_Sis3316_125_0xCC" sheetId="3" r:id="rId3"/>
+    <sheet name="Hard_SIS3316_125" sheetId="2" r:id="rId2"/>
+    <sheet name="Cal_SIS3316_125" sheetId="3" r:id="rId3"/>
     <sheet name="Condition" sheetId="4" r:id="rId4"/>
     <sheet name="Groups" sheetId="5" r:id="rId5"/>
   </sheets>
@@ -50,7 +50,7 @@
     <t>Sync Method</t>
   </si>
   <si>
-    <t>Sis3316_125_0xCC</t>
+    <t>SIS3316_125</t>
   </si>
   <si>
     <t>SIS3316</t>
@@ -59,7 +59,7 @@
     <t>192.168.10.12</t>
   </si>
   <si>
-    <t>Internal</t>
+    <t>LEMO</t>
   </si>
   <si>
     <t>Channels</t>
@@ -890,7 +890,7 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -902,7 +902,7 @@
         <v>13</v>
       </c>
       <c r="H3">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="I3">
         <v>1000000</v>
@@ -1186,28 +1186,28 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>15</v>
       </c>
       <c r="G4">
-        <v>1800</v>
+        <v>700</v>
       </c>
       <c r="H4">
-        <v>350</v>
+        <v>220</v>
       </c>
       <c r="I4">
         <v>1000</v>
       </c>
       <c r="J4">
-        <v>220</v>
+        <v>100</v>
       </c>
       <c r="K4">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="L4">
-        <v>30000</v>
+        <v>260000</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -1219,7 +1219,7 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -1251,17 +1251,17 @@
       <c r="Z4">
         <v>2</v>
       </c>
-      <c r="AA4" t="b">
+      <c r="AA4">
         <v>0</v>
       </c>
       <c r="AB4">
-        <v>50000</v>
+        <v>55000</v>
       </c>
       <c r="AC4">
         <v>1</v>
       </c>
       <c r="AD4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE4">
         <v>0</v>
@@ -1276,7 +1276,7 @@
         <v>1</v>
       </c>
       <c r="AI4">
-        <v>300000</v>
+        <v>800000</v>
       </c>
       <c r="AJ4">
         <v>0</v>
@@ -1371,13 +1371,13 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>15</v>
       </c>
       <c r="G5">
-        <v>530</v>
+        <v>620</v>
       </c>
       <c r="H5" t="s">
         <v>78</v>
@@ -1386,13 +1386,13 @@
         <v>78</v>
       </c>
       <c r="J5">
-        <v>220</v>
+        <v>100</v>
       </c>
       <c r="K5">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="L5">
-        <v>30000</v>
+        <v>500000</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -1436,17 +1436,17 @@
       <c r="Z5">
         <v>2</v>
       </c>
-      <c r="AA5" t="b">
+      <c r="AA5">
         <v>0</v>
       </c>
       <c r="AB5">
-        <v>50000</v>
+        <v>55400</v>
       </c>
       <c r="AC5">
         <v>1</v>
       </c>
       <c r="AD5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE5">
         <v>0</v>
@@ -1461,7 +1461,7 @@
         <v>1</v>
       </c>
       <c r="AI5">
-        <v>300000</v>
+        <v>800000</v>
       </c>
       <c r="AJ5">
         <v>0</v>
@@ -1556,13 +1556,13 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>15</v>
       </c>
       <c r="G6">
-        <v>700</v>
+        <v>640</v>
       </c>
       <c r="H6" t="s">
         <v>78</v>
@@ -1571,13 +1571,13 @@
         <v>78</v>
       </c>
       <c r="J6">
-        <v>220</v>
+        <v>100</v>
       </c>
       <c r="K6">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="L6">
-        <v>30000</v>
+        <v>260000</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1621,17 +1621,17 @@
       <c r="Z6">
         <v>2</v>
       </c>
-      <c r="AA6" t="b">
+      <c r="AA6">
         <v>0</v>
       </c>
       <c r="AB6">
-        <v>50000</v>
+        <v>55400</v>
       </c>
       <c r="AC6">
         <v>1</v>
       </c>
       <c r="AD6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE6">
         <v>0</v>
@@ -1646,7 +1646,7 @@
         <v>1</v>
       </c>
       <c r="AI6">
-        <v>300000</v>
+        <v>800000</v>
       </c>
       <c r="AJ6">
         <v>0</v>
@@ -1741,13 +1741,13 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="F7">
         <v>15</v>
       </c>
       <c r="G7">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="H7" t="s">
         <v>78</v>
@@ -1756,13 +1756,13 @@
         <v>78</v>
       </c>
       <c r="J7">
-        <v>220</v>
+        <v>100</v>
       </c>
       <c r="K7">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="L7">
-        <v>30000</v>
+        <v>500000</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1806,17 +1806,17 @@
       <c r="Z7">
         <v>2</v>
       </c>
-      <c r="AA7" t="b">
+      <c r="AA7">
         <v>0</v>
       </c>
       <c r="AB7">
-        <v>50000</v>
+        <v>55500</v>
       </c>
       <c r="AC7">
         <v>1</v>
       </c>
       <c r="AD7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE7">
         <v>0</v>
@@ -1831,7 +1831,7 @@
         <v>1</v>
       </c>
       <c r="AI7">
-        <v>300000</v>
+        <v>800000</v>
       </c>
       <c r="AJ7">
         <v>0</v>
@@ -2001,10 +2001,10 @@
         <v>15000</v>
       </c>
       <c r="I3">
-        <v>0.0467447368421052</v>
+        <v>0.0472684873949579</v>
       </c>
       <c r="J3">
-        <v>-34.39058171745157</v>
+        <v>-39.32352941176467</v>
       </c>
       <c r="K3" t="s">
         <v>97</v>
@@ -2036,10 +2036,10 @@
         <v>15000</v>
       </c>
       <c r="I4">
-        <v>0.0432688461538461</v>
+        <v>0.0438307792207792</v>
       </c>
       <c r="J4">
-        <v>-27.18076923076924</v>
+        <v>-38.2000000000001</v>
       </c>
       <c r="K4" t="s">
         <v>97</v>
@@ -2071,10 +2071,10 @@
         <v>15000</v>
       </c>
       <c r="I5">
-        <v>0.0238513780918727</v>
+        <v>0.0241069285714285</v>
       </c>
       <c r="J5">
-        <v>-39.81978798586567</v>
+        <v>-46.79500000000002</v>
       </c>
       <c r="K5" t="s">
         <v>97</v>
@@ -2106,10 +2106,10 @@
         <v>15000</v>
       </c>
       <c r="I6">
-        <v>0.0248342163355408</v>
+        <v>0.0251113839285714</v>
       </c>
       <c r="J6">
-        <v>-23.40066225165566</v>
+        <v>-29.84375000000003</v>
       </c>
       <c r="K6" t="s">
         <v>97</v>
@@ -2209,7 +2209,7 @@
         <v>600000</v>
       </c>
       <c r="K3">
-        <v>1.6E-07</v>
+        <v>4E-09</v>
       </c>
       <c r="L3" t="s">
         <v>115</v>
@@ -2302,7 +2302,7 @@
         <v>100000</v>
       </c>
       <c r="K6">
-        <v>2.666666666666667E-09</v>
+        <v>6.666666666666667E-11</v>
       </c>
       <c r="L6" t="s">
         <v>118</v>
@@ -2395,7 +2395,7 @@
         <v>10000</v>
       </c>
       <c r="K9">
-        <v>1.777777777777778E-10</v>
+        <v>4.444444444444445E-12</v>
       </c>
       <c r="L9" t="s">
         <v>121</v>
@@ -2488,7 +2488,7 @@
         <v>5000</v>
       </c>
       <c r="K12">
-        <v>8.888888888888889E-11</v>
+        <v>2.222222222222222E-12</v>
       </c>
       <c r="L12" t="s">
         <v>124</v>
@@ -2581,7 +2581,7 @@
         <v>2500</v>
       </c>
       <c r="K15">
-        <v>4.444444444444444E-11</v>
+        <v>1.111111111111111E-12</v>
       </c>
       <c r="L15" t="s">
         <v>127</v>
@@ -2674,7 +2674,7 @@
         <v>600000</v>
       </c>
       <c r="K18">
-        <v>1.6E-07</v>
+        <v>4E-09</v>
       </c>
       <c r="L18" t="s">
         <v>115</v>
@@ -2767,7 +2767,7 @@
         <v>100000</v>
       </c>
       <c r="K21">
-        <v>2.666666666666667E-09</v>
+        <v>6.666666666666667E-11</v>
       </c>
       <c r="L21" t="s">
         <v>118</v>
@@ -2860,7 +2860,7 @@
         <v>10000</v>
       </c>
       <c r="K24">
-        <v>1.777777777777778E-10</v>
+        <v>4.444444444444445E-12</v>
       </c>
       <c r="L24" t="s">
         <v>121</v>
@@ -2953,7 +2953,7 @@
         <v>5000</v>
       </c>
       <c r="K27">
-        <v>8.888888888888889E-11</v>
+        <v>2.222222222222222E-12</v>
       </c>
       <c r="L27" t="s">
         <v>124</v>
@@ -3046,7 +3046,7 @@
         <v>2500</v>
       </c>
       <c r="K30">
-        <v>4.444444444444444E-11</v>
+        <v>1.111111111111111E-12</v>
       </c>
       <c r="L30" t="s">
         <v>127</v>
@@ -3139,7 +3139,7 @@
         <v>600000</v>
       </c>
       <c r="K33">
-        <v>1.6E-07</v>
+        <v>4E-09</v>
       </c>
       <c r="L33" t="s">
         <v>115</v>
@@ -3232,7 +3232,7 @@
         <v>100000</v>
       </c>
       <c r="K36">
-        <v>2.666666666666667E-09</v>
+        <v>6.666666666666667E-11</v>
       </c>
       <c r="L36" t="s">
         <v>118</v>
@@ -3325,7 +3325,7 @@
         <v>10000</v>
       </c>
       <c r="K39">
-        <v>1.777777777777778E-10</v>
+        <v>4.444444444444445E-12</v>
       </c>
       <c r="L39" t="s">
         <v>121</v>
@@ -3418,7 +3418,7 @@
         <v>5000</v>
       </c>
       <c r="K42">
-        <v>8.888888888888889E-11</v>
+        <v>2.222222222222222E-12</v>
       </c>
       <c r="L42" t="s">
         <v>124</v>
@@ -3511,7 +3511,7 @@
         <v>2500</v>
       </c>
       <c r="K45">
-        <v>4.444444444444444E-11</v>
+        <v>1.111111111111111E-12</v>
       </c>
       <c r="L45" t="s">
         <v>127</v>
@@ -3604,7 +3604,7 @@
         <v>600000</v>
       </c>
       <c r="K48">
-        <v>1.6E-07</v>
+        <v>4E-09</v>
       </c>
       <c r="L48" t="s">
         <v>115</v>
@@ -3697,7 +3697,7 @@
         <v>100000</v>
       </c>
       <c r="K51">
-        <v>2.666666666666667E-09</v>
+        <v>6.666666666666667E-11</v>
       </c>
       <c r="L51" t="s">
         <v>118</v>
@@ -3790,7 +3790,7 @@
         <v>10000</v>
       </c>
       <c r="K54">
-        <v>1.777777777777778E-10</v>
+        <v>4.444444444444445E-12</v>
       </c>
       <c r="L54" t="s">
         <v>121</v>
@@ -3883,7 +3883,7 @@
         <v>5000</v>
       </c>
       <c r="K57">
-        <v>8.888888888888889E-11</v>
+        <v>2.222222222222222E-12</v>
       </c>
       <c r="L57" t="s">
         <v>124</v>
@@ -3976,7 +3976,7 @@
         <v>2500</v>
       </c>
       <c r="K60">
-        <v>4.444444444444444E-11</v>
+        <v>1.111111111111111E-12</v>
       </c>
       <c r="L60" t="s">
         <v>127</v>

</xml_diff>